<commit_message>
Updated graphs with correct trendlines
A1 is big theta n^3
A2 is big O n^3, big Omega n
A3 is big theta n
</commit_message>
<xml_diff>
--- a/p1/graph.xlsx
+++ b/p1/graph.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="graph" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -616,13 +616,14 @@
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.24506786041782"/>
-                  <c:y val="1.3173605188520201E-2"/>
+                  <c:x val="-9.7077994410224092E-2"/>
+                  <c:y val="9.8150829383102933E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -752,13 +753,14 @@
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.1329358649188257"/>
-                  <c:y val="4.5679604910847105E-2"/>
+                  <c:x val="0.21109426362618561"/>
+                  <c:y val="0.16507454200466756"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -893,8 +895,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.36348242117838653"/>
-                  <c:y val="0.22252801523235288"/>
+                  <c:x val="-0.34324064619254513"/>
+                  <c:y val="0.17353193571206621"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1025,11 +1027,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="45096960"/>
-        <c:axId val="45069824"/>
+        <c:axId val="45098880"/>
+        <c:axId val="45109632"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="45096960"/>
+        <c:axId val="45098880"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1062,12 +1064,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45069824"/>
-        <c:crossesAt val="1.0000000000000002E-4"/>
+        <c:crossAx val="45109632"/>
+        <c:crossesAt val="1.0000000000000005E-4"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45069824"/>
+        <c:axId val="45109632"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -1099,7 +1101,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45096960"/>
+        <c:crossAx val="45098880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1112,7 +1114,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1133,7 +1135,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Log-Log</a:t>
+              <a:t>Linear-Linear</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -1167,13 +1169,14 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:trendline>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.49355734230984333"/>
-                  <c:y val="-9.094058456798694E-2"/>
+                  <c:x val="-0.30150823360318824"/>
+                  <c:y val="-7.750649556714731E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1303,13 +1306,14 @@
                 <a:prstDash val="solid"/>
               </a:ln>
             </c:spPr>
-            <c:trendlineType val="power"/>
+            <c:trendlineType val="poly"/>
+            <c:order val="3"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.26864873135605016"/>
-                  <c:y val="9.0419616943348075E-2"/>
+                  <c:x val="-5.8606933773091653E-2"/>
+                  <c:y val="8.7061094693138164E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1444,8 +1448,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.1937708106875155"/>
-                  <c:y val="-3.8063164018855324E-2"/>
+                  <c:x val="0.19377081068751548"/>
+                  <c:y val="-3.8063164018855331E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1576,11 +1580,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="83613568"/>
-        <c:axId val="86147072"/>
+        <c:axId val="61214720"/>
+        <c:axId val="72428544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83613568"/>
+        <c:axId val="61214720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="100"/>
@@ -1612,12 +1616,12 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86147072"/>
-        <c:crossesAt val="1.0000000000000007E-4"/>
+        <c:crossAx val="72428544"/>
+        <c:crossesAt val="1.0000000000000009E-4"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="86147072"/>
+        <c:axId val="72428544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -1649,7 +1653,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83613568"/>
+        <c:crossAx val="61214720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1662,7 +1666,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1673,15 +1677,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>581026</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>131764</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1703,15 +1707,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>465138</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2021,7 +2025,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>